<commit_message>
xiangwei manually add URS
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS交付區/回覆SKL反應問題/IT意見彙總回覆.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS交付區/回覆SKL反應問題/IT意見彙總回覆.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.10.16\St1Share(NAS)\SKL\需求規格書\0.審查意見與回覆\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4C6E541-BFF0-4DD2-AB6C-09391B452022}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{587C2C83-AB37-4364-BCB6-C628D2E99E3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{4140E264-D9EF-438E-8A29-FDC3696D2051}"/>
   </bookViews>
@@ -24,7 +24,7 @@
   </definedNames>
   <calcPr calcId="181029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId4"/>
+    <pivotCache cacheId="5" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="125">
   <si>
     <t>業務大類</t>
   </si>
@@ -401,22 +401,6 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>3/14 UAT已改待L4412相關完成即可測</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>預計 的加總</t>
-  </si>
-  <si>
-    <t>預計</t>
-  </si>
-  <si>
-    <t>實際 的加總</t>
-  </si>
-  <si>
-    <t>實際</t>
-  </si>
-  <si>
     <t>ST1</t>
   </si>
   <si>
@@ -439,6 +423,32 @@
     <t>員工扣薪需條流程、調整流程別判斷與L4511，L4512，L4951同步調整</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
+  <si>
+    <t>廠商環境已測、再排測Dev Online(3/31完成)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>3/25 UAT已改
+L4412相關完成已可測</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>3/14 UAT已改
+L4412相關完成已可測</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>預計 的加總</t>
+  </si>
+  <si>
+    <t>預計</t>
+  </si>
+  <si>
+    <t>實際 的加總</t>
+  </si>
+  <si>
+    <t>實際</t>
+  </si>
 </sst>
 </file>
 
@@ -447,7 +457,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="yyyy/mm/dd;@"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -498,6 +508,13 @@
     <font>
       <sz val="8"/>
       <color theme="1"/>
+      <name val="微軟正黑體"/>
+      <family val="2"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFFF0000"/>
       <name val="微軟正黑體"/>
       <family val="2"/>
       <charset val="136"/>
@@ -607,7 +624,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -746,6 +763,15 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -9503,7 +9529,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Susan Ho" refreshedDate="44635.697189583334" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="18" xr:uid="{CB7BC75C-B3C8-48B8-8E32-8538208DBA3D}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Susan Ho" refreshedDate="44645.473493287034" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="18" xr:uid="{CB7BC75C-B3C8-48B8-8E32-8538208DBA3D}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:U1048576" sheet="IT意見"/>
   </cacheSource>
@@ -9941,10 +9967,11 @@
       <sharedItems containsBlank="1"/>
     </cacheField>
     <cacheField name="預計完成日2" numFmtId="0">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2022-03-09T00:00:00" maxDate="2022-03-26T00:00:00" count="3">
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2022-03-09T00:00:00" maxDate="2022-04-01T00:00:00" count="4">
         <d v="2022-03-09T00:00:00"/>
         <d v="2022-03-25T00:00:00"/>
         <m/>
+        <d v="2022-03-31T00:00:00" u="1"/>
       </sharedItems>
     </cacheField>
     <cacheField name="ST1意見回覆" numFmtId="0">
@@ -9954,7 +9981,7 @@
       <sharedItems containsBlank="1"/>
     </cacheField>
     <cacheField name="實際完成日期" numFmtId="14">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2022-03-02T00:00:00" maxDate="2022-03-16T00:00:00"/>
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2022-03-02T00:00:00" maxDate="2022-03-26T00:00:00"/>
     </cacheField>
     <cacheField name="月" numFmtId="0" databaseField="0">
       <fieldGroup base="13">
@@ -10192,8 +10219,8 @@
     <s v="因L4412建檔尚未完成驗測，故該功能尚未開始"/>
     <x v="0"/>
     <s v="L4041：QC# 1607,1613,1616,1619,1621,1629,1654已改待測"/>
-    <s v="3/14 UAT已改待L4412相關完成即可測"/>
-    <m/>
+    <s v="3/14 UAT已改_x000a_L4412相關完成已可測"/>
+    <d v="2022-03-25T00:00:00"/>
   </r>
   <r>
     <x v="0"/>
@@ -10214,9 +10241,9 @@
     <m/>
     <s v="因L4412建檔尚未完成驗測，故該功能尚未開始"/>
     <x v="1"/>
-    <s v="L4412無誤"/>
-    <s v="L4412：QC# "/>
-    <m/>
+    <s v="待L4412：QC# 調整。 "/>
+    <s v="3/25 UAT已改_x000a_L4412相關完成已可測"/>
+    <d v="2022-03-25T00:00:00"/>
   </r>
   <r>
     <x v="0"/>
@@ -10283,8 +10310,8 @@
     <m/>
     <s v="因L4511問題無法測試"/>
     <x v="1"/>
-    <s v="調整流程別判斷與L4511，L4512，L4951同步調整"/>
-    <m/>
+    <s v="員工扣薪需調整流程別判斷與L4511，L4512，L4951同步調整"/>
+    <s v="廠商環境已測、再排測Dev Online(3/31完成)"/>
     <m/>
   </r>
   <r>
@@ -10306,8 +10333,8 @@
     <m/>
     <s v="因L4511問題無法測試"/>
     <x v="1"/>
-    <s v="調整為明細檔查詢"/>
-    <m/>
+    <s v="員工扣薪需條流程、調整為明細檔查詢"/>
+    <s v="廠商環境已測、再排測Dev Online(3/31完成)"/>
     <m/>
   </r>
   <r>
@@ -10329,8 +10356,8 @@
     <m/>
     <s v="因L4511問題無法測試"/>
     <x v="1"/>
-    <s v="調整為明細檔維護"/>
-    <m/>
+    <s v="員工扣薪需條流程、調整為明細檔維護"/>
+    <s v="廠商環境已測、再排測Dev Online(3/31完成)"/>
     <m/>
   </r>
   <r>
@@ -10352,8 +10379,8 @@
     <m/>
     <s v="無法測試"/>
     <x v="1"/>
-    <s v="調整流程別判斷與L4511，L4512，L4951同步調整"/>
-    <m/>
+    <s v="員工扣薪需條流程、調整流程別判斷與L4511，L4512，L4951同步調整"/>
+    <s v="廠商環境已測、再排測Dev Online(3/31完成)"/>
     <m/>
   </r>
   <r>
@@ -10406,7 +10433,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4CF3A8E3-141C-4D3C-B6C3-AAB6B80D8DF4}" name="樞紐分析表1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="IT意見收到" colHeaderCaption="ST1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4CF3A8E3-141C-4D3C-B6C3-AAB6B80D8DF4}" name="樞紐分析表1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="IT意見收到" colHeaderCaption="ST1">
   <location ref="A3:G7" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="22">
     <pivotField axis="axisRow" showAll="0">
@@ -10805,10 +10832,11 @@
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField axis="axisCol" dataField="1" showAll="0">
-      <items count="4">
+      <items count="5">
         <item x="0"/>
         <item x="1"/>
         <item h="1" x="2"/>
+        <item m="1" x="3"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -10876,7 +10904,7 @@
     <dataField name="預計" fld="17" subtotal="count" baseField="0" baseItem="0"/>
     <dataField name="實際" fld="20" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <pivotTableStyleInfo name="PivotStyleLight21" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
       <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
@@ -11187,8 +11215,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54A8B2F8-F296-46D0-96AF-94187800F03C}">
   <dimension ref="A1:U18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D7" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:U17"/>
+    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="28" defaultRowHeight="13" x14ac:dyDescent="0.35"/>
@@ -11799,7 +11827,7 @@
         <v>44629</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="42" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:21" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A10" s="36">
         <v>44627</v>
       </c>
@@ -11855,11 +11883,13 @@
         <v>111</v>
       </c>
       <c r="T10" s="32" t="s">
-        <v>112</v>
-      </c>
-      <c r="U10" s="28"/>
+        <v>120</v>
+      </c>
+      <c r="U10" s="28">
+        <v>44645</v>
+      </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:21" ht="26" x14ac:dyDescent="0.35">
       <c r="A11" s="36">
         <v>44627</v>
       </c>
@@ -11912,10 +11942,14 @@
         <v>44645</v>
       </c>
       <c r="S11" s="42" t="s">
-        <v>118</v>
-      </c>
-      <c r="T11" s="29"/>
-      <c r="U11" s="28"/>
+        <v>113</v>
+      </c>
+      <c r="T11" s="48" t="s">
+        <v>119</v>
+      </c>
+      <c r="U11" s="28">
+        <v>44645</v>
+      </c>
     </row>
     <row r="12" spans="1:21" ht="26" x14ac:dyDescent="0.35">
       <c r="A12" s="36">
@@ -12100,13 +12134,15 @@
       <c r="Q14" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="R14" s="28">
+      <c r="R14" s="47">
         <v>44645</v>
       </c>
       <c r="S14" s="40" t="s">
-        <v>119</v>
-      </c>
-      <c r="T14" s="30"/>
+        <v>114</v>
+      </c>
+      <c r="T14" s="46" t="s">
+        <v>118</v>
+      </c>
       <c r="U14" s="28"/>
     </row>
     <row r="15" spans="1:21" ht="21" x14ac:dyDescent="0.35">
@@ -12160,13 +12196,15 @@
       <c r="Q15" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="R15" s="28">
+      <c r="R15" s="47">
         <v>44645</v>
       </c>
       <c r="S15" s="42" t="s">
-        <v>120</v>
-      </c>
-      <c r="T15" s="29"/>
+        <v>115</v>
+      </c>
+      <c r="T15" s="46" t="s">
+        <v>118</v>
+      </c>
       <c r="U15" s="28"/>
     </row>
     <row r="16" spans="1:21" ht="21" x14ac:dyDescent="0.35">
@@ -12220,13 +12258,15 @@
       <c r="Q16" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="R16" s="28">
+      <c r="R16" s="47">
         <v>44645</v>
       </c>
       <c r="S16" s="42" t="s">
-        <v>121</v>
-      </c>
-      <c r="T16" s="29"/>
+        <v>116</v>
+      </c>
+      <c r="T16" s="46" t="s">
+        <v>118</v>
+      </c>
       <c r="U16" s="28"/>
     </row>
     <row r="17" spans="1:21" ht="31.5" x14ac:dyDescent="0.35">
@@ -12268,13 +12308,15 @@
       <c r="Q17" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="R17" s="28">
+      <c r="R17" s="47">
         <v>44645</v>
       </c>
       <c r="S17" s="40" t="s">
-        <v>122</v>
-      </c>
-      <c r="T17" s="30"/>
+        <v>117</v>
+      </c>
+      <c r="T17" s="46" t="s">
+        <v>118</v>
+      </c>
       <c r="U17" s="28"/>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.35">
@@ -12297,7 +12339,7 @@
   <dimension ref="A3:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -12309,12 +12351,14 @@
     <col min="5" max="5" width="4.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.78515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B3" s="4" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -12325,10 +12369,10 @@
         <v>44645</v>
       </c>
       <c r="F4" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="G4" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -12336,16 +12380,16 @@
         <v>95</v>
       </c>
       <c r="B5" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="C5" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="D5" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="E5" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
@@ -12356,17 +12400,19 @@
         <v>11</v>
       </c>
       <c r="C6" s="3">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D6" s="3">
         <v>5</v>
       </c>
-      <c r="E6" s="3"/>
+      <c r="E6" s="3">
+        <v>1</v>
+      </c>
       <c r="F6" s="3">
         <v>16</v>
       </c>
       <c r="G6" s="3">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
@@ -12377,17 +12423,19 @@
         <v>11</v>
       </c>
       <c r="C7" s="3">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D7" s="3">
         <v>5</v>
       </c>
-      <c r="E7" s="3"/>
+      <c r="E7" s="3">
+        <v>1</v>
+      </c>
       <c r="F7" s="3">
         <v>16</v>
       </c>
       <c r="G7" s="3">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>